<commit_message>
Now the data from WitMotion is more believable and better matches theoretical data
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/H/AngVel/f10RPM/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/H/AngVel/f10RPM/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adg66\Downloads\PMKS_Verification\Mechanisms\Four_Bar_Mechanism\TeachingLab_Four_Bar\RMSE_Results\H\AngVel\f10RPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B39D5B-A423-4258-B20F-BF068DEE5606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF59047-8991-43BC-9503-36C76C8347AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="240" windowWidth="15120" windowHeight="8604" xr2:uid="{25001E0F-8AA5-408A-B4C6-D2C496525E07}"/>
+    <workbookView xWindow="5040" yWindow="240" windowWidth="15120" windowHeight="8604" xr2:uid="{75CBA699-D3B0-42E8-95A0-470D93008DFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A771449-7016-4467-A8C7-919F7D90E773}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFCD2A5-8DE9-4081-9798-110376110540}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -410,7 +410,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>23.41363837464225</v>
+        <v>0.80528920756096667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>